<commit_message>
add data folder and update scripts
</commit_message>
<xml_diff>
--- a/data_description.xlsx
+++ b/data_description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ap4818/Documents/bal_revision_github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artemispapadaki/Documents/bal_revision_github_sent_to_jack/BAL_proteomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820CEA71-6135-1F42-A7DA-BD44C21232E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C382E4A-9DEF-2944-AE4C-84BA4A3F16BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="1220" windowWidth="26440" windowHeight="14420" xr2:uid="{2C8C340F-179E-B047-83DB-7506D35467CE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Column Name</t>
   </si>
@@ -167,7 +167,13 @@
     <t>Plasma Flow data (file: plasma_long_personal_clinical_flow.csv)</t>
   </si>
   <si>
-    <t>columns include the flow data: EA to FI, self descriptive</t>
+    <t>GeneID2</t>
+  </si>
+  <si>
+    <t>GeneID, combined with panel information, associated with each protein</t>
+  </si>
+  <si>
+    <t>columns include the flow data: X to BD, self descriptive</t>
   </si>
 </sst>
 </file>
@@ -644,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C778E8B5-8BB5-064E-949A-B9450BE1E6ED}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,20 +739,26 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
@@ -832,22 +844,22 @@
         <v>28</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>